<commit_message>
reading qs - replaced concept with text column
</commit_message>
<xml_diff>
--- a/resources/affect_reading_questions/causalclaims_rote_questions.xlsx
+++ b/resources/affect_reading_questions/causalclaims_rote_questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roso8920\Dropbox (Emotive Computing)\Misc\FENIX\stroop-psychopy\resources\affect_reading_questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9767418-3218-444A-B2C1-DDB5E1071FE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE69985-294F-4793-99FC-23524D0A729C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29230" yWindow="-5380" windowWidth="25370" windowHeight="14890" xr2:uid="{AEEF95D1-22C9-4D65-99EA-C3712770BD16}"/>
+    <workbookView xWindow="19870" yWindow="-7920" windowWidth="21140" windowHeight="12410" xr2:uid="{AEEF95D1-22C9-4D65-99EA-C3712770BD16}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
-  <si>
-    <t>Quasi-Experimental Design</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Please select the best answer to the question.</t>
   </si>
@@ -86,9 +83,6 @@
     <t>Being on sports teams</t>
   </si>
   <si>
-    <t>Experimental Design</t>
-  </si>
-  <si>
     <t>Experiments which observe effects on an already-defined categorization of people are called</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>PageNum</t>
   </si>
   <si>
-    <t>Concept</t>
-  </si>
-  <si>
     <t>InstructionText</t>
   </si>
   <si>
@@ -126,6 +117,12 @@
   </si>
   <si>
     <t>CorrectAnswer</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>causalclaims</t>
   </si>
 </sst>
 </file>
@@ -480,35 +477,35 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="A6:J11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -516,25 +513,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -542,25 +539,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
       <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -568,25 +565,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
       <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -594,25 +591,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>